<commit_message>
Adicionados M7 e M9 no DataFrame
</commit_message>
<xml_diff>
--- a/docs/Projeto/analytics-raw-data/metrics_df.xlsx
+++ b/docs/Projeto/analytics-raw-data/metrics_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,25 +451,35 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>m7</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>m9</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>repository</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>asc1</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>ac1</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>total</t>
         </is>
@@ -485,23 +495,29 @@
       <c r="C2" t="n">
         <v>0.9444444444444444</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="D2" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>v1.0.0</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>0.3666666666666666</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>0.3666666666666666</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>0.3666666666666666</v>
       </c>
     </row>
@@ -515,23 +531,29 @@
       <c r="C3" t="n">
         <v>0.9444444444444444</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
+      <c r="D3" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>v1.1.0</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
         <v>0.3666666666666666</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>0.3666666666666666</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>0.3666666666666666</v>
       </c>
     </row>
@@ -545,23 +567,29 @@
       <c r="C4" t="n">
         <v>0.9411764705882353</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
+      <c r="D4" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E4" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>v1.10.0</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>0.3882352941176471</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.3882352941176471</v>
-      </c>
       <c r="H4" t="n">
+        <v>0.3882352941176471</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.3882352941176471</v>
+      </c>
+      <c r="J4" t="n">
         <v>0.3882352941176471</v>
       </c>
     </row>
@@ -575,23 +603,29 @@
       <c r="C5" t="n">
         <v>0.9411764705882353</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
+      <c r="D5" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>v1.10.2</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>0.3882352941176471</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.3882352941176471</v>
-      </c>
       <c r="H5" t="n">
+        <v>0.3882352941176471</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.3882352941176471</v>
+      </c>
+      <c r="J5" t="n">
         <v>0.3882352941176471</v>
       </c>
     </row>
@@ -605,23 +639,29 @@
       <c r="C6" t="n">
         <v>0.9411764705882353</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
+      <c r="D6" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>v1.10.3</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>0.3882352941176471</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.3882352941176471</v>
-      </c>
       <c r="H6" t="n">
+        <v>0.3882352941176471</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.3882352941176471</v>
+      </c>
+      <c r="J6" t="n">
         <v>0.3882352941176471</v>
       </c>
     </row>
@@ -635,23 +675,29 @@
       <c r="C7" t="n">
         <v>0.9365079365079365</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
+      <c r="D7" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>v1.4.0</t>
         </is>
       </c>
-      <c r="F7" t="n">
+      <c r="H7" t="n">
         <v>0.3823809523809524</v>
       </c>
-      <c r="G7" t="n">
+      <c r="I7" t="n">
         <v>0.3823809523809524</v>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
         <v>0.3823809523809524</v>
       </c>
     </row>
@@ -665,23 +711,29 @@
       <c r="C8" t="n">
         <v>0.9365079365079365</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
+      <c r="D8" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E8" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>v1.5.0</t>
         </is>
       </c>
-      <c r="F8" t="n">
+      <c r="H8" t="n">
         <v>0.3823809523809524</v>
       </c>
-      <c r="G8" t="n">
+      <c r="I8" t="n">
         <v>0.3823809523809524</v>
       </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
         <v>0.3823809523809524</v>
       </c>
     </row>
@@ -695,23 +747,29 @@
       <c r="C9" t="n">
         <v>0.9365079365079365</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
+      <c r="D9" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E9" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>v1.6.0</t>
         </is>
       </c>
-      <c r="F9" t="n">
-        <v>0.3876190476190476</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.3876190476190476</v>
-      </c>
       <c r="H9" t="n">
+        <v>0.3876190476190476</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.3876190476190476</v>
+      </c>
+      <c r="J9" t="n">
         <v>0.3876190476190476</v>
       </c>
     </row>
@@ -725,23 +783,29 @@
       <c r="C10" t="n">
         <v>0.9365079365079365</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
+      <c r="D10" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>v1.7.0</t>
         </is>
       </c>
-      <c r="F10" t="n">
-        <v>0.3876190476190476</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.3876190476190476</v>
-      </c>
       <c r="H10" t="n">
+        <v>0.3876190476190476</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.3876190476190476</v>
+      </c>
+      <c r="J10" t="n">
         <v>0.3876190476190476</v>
       </c>
     </row>
@@ -755,23 +819,29 @@
       <c r="C11" t="n">
         <v>0.9365079365079365</v>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
+      <c r="D11" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E11" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>v1.7.1</t>
         </is>
       </c>
-      <c r="F11" t="n">
-        <v>0.3876190476190476</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.3876190476190476</v>
-      </c>
       <c r="H11" t="n">
+        <v>0.3876190476190476</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.3876190476190476</v>
+      </c>
+      <c r="J11" t="n">
         <v>0.3876190476190476</v>
       </c>
     </row>
@@ -785,23 +855,29 @@
       <c r="C12" t="n">
         <v>0.9365079365079365</v>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
+      <c r="D12" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E12" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>v1.7.2</t>
         </is>
       </c>
-      <c r="F12" t="n">
-        <v>0.3876190476190476</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.3876190476190476</v>
-      </c>
       <c r="H12" t="n">
+        <v>0.3876190476190476</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.3876190476190476</v>
+      </c>
+      <c r="J12" t="n">
         <v>0.3876190476190476</v>
       </c>
     </row>
@@ -815,23 +891,29 @@
       <c r="C13" t="n">
         <v>0.9365079365079365</v>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
+      <c r="D13" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E13" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>v1.7.3</t>
         </is>
       </c>
-      <c r="F13" t="n">
-        <v>0.3876190476190476</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.3876190476190476</v>
-      </c>
       <c r="H13" t="n">
+        <v>0.3876190476190476</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.3876190476190476</v>
+      </c>
+      <c r="J13" t="n">
         <v>0.3876190476190476</v>
       </c>
     </row>
@@ -845,23 +927,29 @@
       <c r="C14" t="n">
         <v>0.9411764705882353</v>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
+      <c r="D14" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E14" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t>v1.8.0</t>
         </is>
       </c>
-      <c r="F14" t="n">
-        <v>0.3882352941176471</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.3882352941176471</v>
-      </c>
       <c r="H14" t="n">
+        <v>0.3882352941176471</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.3882352941176471</v>
+      </c>
+      <c r="J14" t="n">
         <v>0.3882352941176471</v>
       </c>
     </row>
@@ -875,23 +963,29 @@
       <c r="C15" t="n">
         <v>0.9411764705882353</v>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
+      <c r="D15" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E15" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
         <is>
           <t>v1.9.0</t>
         </is>
       </c>
-      <c r="F15" t="n">
-        <v>0.3882352941176471</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.3882352941176471</v>
-      </c>
       <c r="H15" t="n">
+        <v>0.3882352941176471</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.3882352941176471</v>
+      </c>
+      <c r="J15" t="n">
         <v>0.3882352941176471</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adicionado json das última release
</commit_message>
<xml_diff>
--- a/docs/Projeto/analytics-raw-data/metrics_df.xlsx
+++ b/docs/Projeto/analytics-raw-data/metrics_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,13 +487,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.09259259259259259</v>
+        <v>0.875</v>
       </c>
       <c r="B2" t="n">
-        <v>0.07407407407407407</v>
+        <v>0.125</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>79.31</v>
@@ -508,28 +508,28 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>v1.0.0</t>
+          <t>v1.00.0</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0.3666666666666666</v>
+        <v>0.66</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3666666666666666</v>
+        <v>0.66</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3666666666666666</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.09259259259259259</v>
+        <v>0.875</v>
       </c>
       <c r="B3" t="n">
-        <v>0.07407407407407407</v>
+        <v>0.125</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>79.31</v>
@@ -544,28 +544,28 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>v1.1.0</t>
+          <t>v1.01.0</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0.3666666666666666</v>
+        <v>0.66</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3666666666666666</v>
+        <v>0.66</v>
       </c>
       <c r="J3" t="n">
-        <v>0.3666666666666666</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.1764705882352941</v>
+        <v>0.9</v>
       </c>
       <c r="B4" t="n">
-        <v>0.05882352941176471</v>
+        <v>0.1</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9411764705882353</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
         <v>79.31</v>
@@ -580,28 +580,28 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>v1.10.0</t>
+          <t>v1.04.0</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="I4" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6600000000000001</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.1764705882352941</v>
+        <v>0.9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.05882352941176471</v>
+        <v>0.1</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9411764705882353</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>79.31</v>
@@ -616,28 +616,28 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>v1.10.2</t>
+          <t>v1.05.0</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6600000000000001</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.1764705882352941</v>
+        <v>0.9</v>
       </c>
       <c r="B6" t="n">
-        <v>0.05882352941176471</v>
+        <v>0.1</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9411764705882353</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
         <v>79.31</v>
@@ -652,28 +652,28 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>v1.10.3</t>
+          <t>v1.06.0</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="I6" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6600000000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.1587301587301587</v>
+        <v>0.9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.06349206349206349</v>
+        <v>0.1</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9365079365079365</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>79.31</v>
@@ -688,28 +688,28 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>v1.4.0</t>
+          <t>v1.07.0</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>0.3823809523809524</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="I7" t="n">
-        <v>0.3823809523809524</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="J7" t="n">
-        <v>0.3823809523809524</v>
+        <v>0.6600000000000001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.1587301587301587</v>
+        <v>0.9</v>
       </c>
       <c r="B8" t="n">
-        <v>0.06349206349206349</v>
+        <v>0.1</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9365079365079365</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
         <v>79.31</v>
@@ -724,28 +724,28 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>v1.5.0</t>
+          <t>v1.07.1</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>0.3823809523809524</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="I8" t="n">
-        <v>0.3823809523809524</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="J8" t="n">
-        <v>0.3823809523809524</v>
+        <v>0.6600000000000001</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.1746031746031746</v>
+        <v>0.9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.06349206349206349</v>
+        <v>0.1</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9365079365079365</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
         <v>79.31</v>
@@ -760,28 +760,28 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>v1.6.0</t>
+          <t>v1.07.2</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="I9" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6600000000000001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.1746031746031746</v>
+        <v>0.9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.06349206349206349</v>
+        <v>0.1</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9365079365079365</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
         <v>79.31</v>
@@ -796,28 +796,28 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>v1.7.0</t>
+          <t>v1.07.3</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="I10" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="J10" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6600000000000001</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.1746031746031746</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="B11" t="n">
-        <v>0.06349206349206349</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9365079365079365</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
         <v>79.31</v>
@@ -832,28 +832,28 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>v1.7.1</t>
+          <t>v1.08.0</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6300000000000001</v>
       </c>
       <c r="I11" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6300000000000001</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6300000000000001</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.1746031746031746</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="B12" t="n">
-        <v>0.06349206349206349</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9365079365079365</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
         <v>79.31</v>
@@ -868,28 +868,28 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>v1.7.2</t>
+          <t>v1.09.0</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6325000000000001</v>
       </c>
       <c r="I12" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6325000000000001</v>
       </c>
       <c r="J12" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6325000000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.1746031746031746</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="B13" t="n">
-        <v>0.06349206349206349</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9365079365079365</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
         <v>79.31</v>
@@ -904,28 +904,28 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>v1.7.3</t>
+          <t>v1.10.0</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6346153846153846</v>
       </c>
       <c r="I13" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6346153846153846</v>
       </c>
       <c r="J13" t="n">
-        <v>0.3876190476190476</v>
+        <v>0.6346153846153846</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.1764705882352941</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="B14" t="n">
-        <v>0.05882352941176471</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9411764705882353</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
         <v>79.31</v>
@@ -940,28 +940,28 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>v1.8.0</t>
+          <t>v1.10.2</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6346153846153846</v>
       </c>
       <c r="I14" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6346153846153846</v>
       </c>
       <c r="J14" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6346153846153846</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.1764705882352941</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="B15" t="n">
-        <v>0.05882352941176471</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9411764705882353</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
         <v>79.31</v>
@@ -976,17 +976,89 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>v1.9.0</t>
+          <t>v1.10.3</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6346153846153846</v>
       </c>
       <c r="I15" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6346153846153846</v>
       </c>
       <c r="J15" t="n">
-        <v>0.3882352941176471</v>
+        <v>0.6346153846153846</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0.8461538461538461</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.07692307692307693</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E16" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>v1.11.0</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>0.6346153846153846</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.6346153846153846</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.6346153846153846</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>0.8421052631578947</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.05263157894736842</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.868421052631579</v>
+      </c>
+      <c r="D17" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E17" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>v2.00.0</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>0.5818421052631579</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.5818421052631579</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.5818421052631579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorganizada células e gráficos do notebook
</commit_message>
<xml_diff>
--- a/docs/Projeto/analytics-raw-data/metrics_df.xlsx
+++ b/docs/Projeto/analytics-raw-data/metrics_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,35 +451,25 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>m7</t>
+          <t>repository</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>m9</t>
+          <t>version</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>repository</t>
+          <t>asc1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>version</t>
+          <t>ac1</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>asc1</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>ac1</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>total</t>
         </is>
@@ -495,29 +485,23 @@
       <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E2" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>v1.00.0</t>
         </is>
       </c>
+      <c r="F2" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.66</v>
+      </c>
       <c r="H2" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="J2" t="n">
         <v>0.66</v>
       </c>
     </row>
@@ -531,29 +515,23 @@
       <c r="C3" t="n">
         <v>1</v>
       </c>
-      <c r="D3" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E3" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>v1.01.0</t>
         </is>
       </c>
+      <c r="F3" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.66</v>
+      </c>
       <c r="H3" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="J3" t="n">
         <v>0.66</v>
       </c>
     </row>
@@ -567,29 +545,23 @@
       <c r="C4" t="n">
         <v>1</v>
       </c>
-      <c r="D4" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E4" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>v1.04.0</t>
         </is>
       </c>
+      <c r="F4" t="n">
+        <v>0.6600000000000001</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.6600000000000001</v>
+      </c>
       <c r="H4" t="n">
-        <v>0.6600000000000001</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.6600000000000001</v>
-      </c>
-      <c r="J4" t="n">
         <v>0.6600000000000001</v>
       </c>
     </row>
@@ -603,29 +575,23 @@
       <c r="C5" t="n">
         <v>1</v>
       </c>
-      <c r="D5" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E5" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>v1.05.0</t>
         </is>
       </c>
+      <c r="F5" t="n">
+        <v>0.6600000000000001</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.6600000000000001</v>
+      </c>
       <c r="H5" t="n">
-        <v>0.6600000000000001</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.6600000000000001</v>
-      </c>
-      <c r="J5" t="n">
         <v>0.6600000000000001</v>
       </c>
     </row>
@@ -639,29 +605,23 @@
       <c r="C6" t="n">
         <v>1</v>
       </c>
-      <c r="D6" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E6" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>v1.06.0</t>
         </is>
       </c>
+      <c r="F6" t="n">
+        <v>0.6600000000000001</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.6600000000000001</v>
+      </c>
       <c r="H6" t="n">
-        <v>0.6600000000000001</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.6600000000000001</v>
-      </c>
-      <c r="J6" t="n">
         <v>0.6600000000000001</v>
       </c>
     </row>
@@ -675,29 +635,23 @@
       <c r="C7" t="n">
         <v>1</v>
       </c>
-      <c r="D7" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E7" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>v1.07.0</t>
         </is>
       </c>
+      <c r="F7" t="n">
+        <v>0.6600000000000001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.6600000000000001</v>
+      </c>
       <c r="H7" t="n">
-        <v>0.6600000000000001</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.6600000000000001</v>
-      </c>
-      <c r="J7" t="n">
         <v>0.6600000000000001</v>
       </c>
     </row>
@@ -711,29 +665,23 @@
       <c r="C8" t="n">
         <v>1</v>
       </c>
-      <c r="D8" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E8" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>v1.07.1</t>
         </is>
       </c>
+      <c r="F8" t="n">
+        <v>0.6600000000000001</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.6600000000000001</v>
+      </c>
       <c r="H8" t="n">
-        <v>0.6600000000000001</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.6600000000000001</v>
-      </c>
-      <c r="J8" t="n">
         <v>0.6600000000000001</v>
       </c>
     </row>
@@ -747,29 +695,23 @@
       <c r="C9" t="n">
         <v>1</v>
       </c>
-      <c r="D9" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E9" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>v1.07.2</t>
         </is>
       </c>
+      <c r="F9" t="n">
+        <v>0.6600000000000001</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.6600000000000001</v>
+      </c>
       <c r="H9" t="n">
-        <v>0.6600000000000001</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.6600000000000001</v>
-      </c>
-      <c r="J9" t="n">
         <v>0.6600000000000001</v>
       </c>
     </row>
@@ -783,29 +725,23 @@
       <c r="C10" t="n">
         <v>1</v>
       </c>
-      <c r="D10" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E10" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>v1.07.3</t>
         </is>
       </c>
+      <c r="F10" t="n">
+        <v>0.6600000000000001</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.6600000000000001</v>
+      </c>
       <c r="H10" t="n">
-        <v>0.6600000000000001</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.6600000000000001</v>
-      </c>
-      <c r="J10" t="n">
         <v>0.6600000000000001</v>
       </c>
     </row>
@@ -819,29 +755,23 @@
       <c r="C11" t="n">
         <v>1</v>
       </c>
-      <c r="D11" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E11" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>v1.08.0</t>
         </is>
       </c>
+      <c r="F11" t="n">
+        <v>0.6300000000000001</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.6300000000000001</v>
+      </c>
       <c r="H11" t="n">
-        <v>0.6300000000000001</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.6300000000000001</v>
-      </c>
-      <c r="J11" t="n">
         <v>0.6300000000000001</v>
       </c>
     </row>
@@ -855,29 +785,23 @@
       <c r="C12" t="n">
         <v>1</v>
       </c>
-      <c r="D12" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E12" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>v1.09.0</t>
         </is>
       </c>
+      <c r="F12" t="n">
+        <v>0.6325000000000001</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.6325000000000001</v>
+      </c>
       <c r="H12" t="n">
-        <v>0.6325000000000001</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.6325000000000001</v>
-      </c>
-      <c r="J12" t="n">
         <v>0.6325000000000001</v>
       </c>
     </row>
@@ -891,29 +815,23 @@
       <c r="C13" t="n">
         <v>1</v>
       </c>
-      <c r="D13" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E13" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>v1.10.0</t>
         </is>
       </c>
+      <c r="F13" t="n">
+        <v>0.6346153846153846</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.6346153846153846</v>
+      </c>
       <c r="H13" t="n">
-        <v>0.6346153846153846</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.6346153846153846</v>
-      </c>
-      <c r="J13" t="n">
         <v>0.6346153846153846</v>
       </c>
     </row>
@@ -927,29 +845,23 @@
       <c r="C14" t="n">
         <v>1</v>
       </c>
-      <c r="D14" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E14" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>v1.10.2</t>
         </is>
       </c>
+      <c r="F14" t="n">
+        <v>0.6346153846153846</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.6346153846153846</v>
+      </c>
       <c r="H14" t="n">
-        <v>0.6346153846153846</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.6346153846153846</v>
-      </c>
-      <c r="J14" t="n">
         <v>0.6346153846153846</v>
       </c>
     </row>
@@ -963,29 +875,23 @@
       <c r="C15" t="n">
         <v>1</v>
       </c>
-      <c r="D15" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E15" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>v1.10.3</t>
         </is>
       </c>
+      <c r="F15" t="n">
+        <v>0.6346153846153846</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.6346153846153846</v>
+      </c>
       <c r="H15" t="n">
-        <v>0.6346153846153846</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0.6346153846153846</v>
-      </c>
-      <c r="J15" t="n">
         <v>0.6346153846153846</v>
       </c>
     </row>
@@ -999,29 +905,23 @@
       <c r="C16" t="n">
         <v>1</v>
       </c>
-      <c r="D16" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E16" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>v1.11.0</t>
         </is>
       </c>
+      <c r="F16" t="n">
+        <v>0.6346153846153846</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.6346153846153846</v>
+      </c>
       <c r="H16" t="n">
-        <v>0.6346153846153846</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0.6346153846153846</v>
-      </c>
-      <c r="J16" t="n">
         <v>0.6346153846153846</v>
       </c>
     </row>
@@ -1035,29 +935,23 @@
       <c r="C17" t="n">
         <v>0.868421052631579</v>
       </c>
-      <c r="D17" t="n">
-        <v>79.31</v>
-      </c>
-      <c r="E17" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Desenvolvimento</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>v2.00.0</t>
         </is>
       </c>
+      <c r="F17" t="n">
+        <v>0.5818421052631579</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.5818421052631579</v>
+      </c>
       <c r="H17" t="n">
-        <v>0.5818421052631579</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.5818421052631579</v>
-      </c>
-      <c r="J17" t="n">
         <v>0.5818421052631579</v>
       </c>
     </row>

</xml_diff>